<commit_message>
Actualizacion de archivos por nombre incorrecto y agregar acciones correctivas
</commit_message>
<xml_diff>
--- a/Proyectos/Viaticos/02. Planeación/Viaticos-PlanProyecto.xlsx
+++ b/Proyectos/Viaticos/02. Planeación/Viaticos-PlanProyecto.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Generales" sheetId="1" state="visible" r:id="rId2"/>
@@ -182,7 +182,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="154">
   <si>
     <t>Plan de Proyecto</t>
   </si>
@@ -331,7 +331,7 @@
     <t>Mayra Tejeda</t>
   </si>
   <si>
-    <t>Tester</t>
+    <t>Tester/Diseñador</t>
   </si>
   <si>
     <t>mayra.tejeda@gmail.com</t>
@@ -367,7 +367,7 @@
     <t>NO aplica</t>
   </si>
   <si>
-    <t>Equipo del &lt;Cliente&gt;</t>
+    <t>Equipo de Qualtop</t>
   </si>
   <si>
     <t>Rene Pulido</t>
@@ -472,7 +472,7 @@
     <t>Infraestructura</t>
   </si>
   <si>
-    <t>eclipse</t>
+    <t>Ruby</t>
   </si>
   <si>
     <t>internet</t>
@@ -530,6 +530,9 @@
   </si>
   <si>
     <t>Abierto</t>
+  </si>
+  <si>
+    <t>Quincenal</t>
   </si>
   <si>
     <t>Valor</t>
@@ -651,7 +654,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="36">
+  <fonts count="38">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -760,8 +763,14 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial Narrow"/>
+      <color rgb="FF000000"/>
+      <name val="arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -774,6 +783,13 @@
     <font>
       <b val="true"/>
       <sz val="20"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial Narrow"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1434,11 +1450,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="171">
+  <cellXfs count="170">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1583,26 +1599,22 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1643,7 +1655,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1655,7 +1667,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1675,7 +1687,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1695,23 +1707,23 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1735,19 +1747,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="22" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1759,15 +1771,15 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1775,7 +1787,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1783,15 +1795,15 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="30" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="30" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="30" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1815,35 +1827,35 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="6" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="30" fillId="6" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="30" fillId="7" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="30" fillId="7" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="30" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="32" fillId="6" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="32" fillId="6" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="32" fillId="7" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="32" fillId="7" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="32" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1851,19 +1863,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1871,27 +1883,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="8" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="30" fillId="6" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="30" fillId="7" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="4" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="4" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="32" fillId="8" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="32" fillId="6" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="32" fillId="7" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="4" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="4" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="34" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="180" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1911,19 +1923,19 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="8" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="30" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="3" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="3" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="32" fillId="8" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="32" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="3" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="3" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1943,27 +1955,27 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="8" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="30" fillId="8" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="30" fillId="6" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="30" fillId="6" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="32" fillId="8" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="32" fillId="8" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="32" fillId="6" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="32" fillId="6" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="3" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="3" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1971,19 +1983,19 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="8" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="30" fillId="8" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="30" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="30" fillId="8" borderId="42" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="32" fillId="8" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="32" fillId="8" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="32" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="32" fillId="8" borderId="42" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1991,62 +2003,62 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="44" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="45" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="46" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="47" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="44" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="45" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="46" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="47" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2055,11 +2067,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="4" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="4" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2067,11 +2079,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="41" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="34" fillId="0" borderId="41" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2091,15 +2103,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="4" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="7" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="6" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="4" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="7" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="6" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2115,11 +2127,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="8" borderId="50" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="3" borderId="51" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="8" borderId="50" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="3" borderId="51" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2201,15 +2213,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1386000</xdr:colOff>
+      <xdr:colOff>1413000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>1080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>3884040</xdr:colOff>
+      <xdr:colOff>3910680</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>63000</xdr:rowOff>
+      <xdr:rowOff>62640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2222,8 +2234,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4167720" y="1080"/>
-          <a:ext cx="2498040" cy="823680"/>
+          <a:off x="4194720" y="1080"/>
+          <a:ext cx="2497680" cy="823320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2243,15 +2255,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>405000</xdr:colOff>
+      <xdr:colOff>432000</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>163440</xdr:rowOff>
+      <xdr:rowOff>154440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>405360</xdr:colOff>
+      <xdr:colOff>432360</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>163800</xdr:rowOff>
+      <xdr:rowOff>154800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2260,7 +2272,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8216640" y="1020600"/>
+          <a:off x="8243640" y="1011600"/>
           <a:ext cx="360" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -2286,15 +2298,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>900000</xdr:colOff>
+      <xdr:colOff>927000</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>163080</xdr:rowOff>
+      <xdr:rowOff>154080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>79560</xdr:colOff>
+      <xdr:colOff>106200</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>163440</xdr:rowOff>
+      <xdr:rowOff>154440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2303,8 +2315,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4964400" y="1020240"/>
-          <a:ext cx="5390640" cy="360"/>
+          <a:off x="4991400" y="1011240"/>
+          <a:ext cx="5390280" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2326,15 +2338,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>405000</xdr:colOff>
+      <xdr:colOff>432000</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>294840</xdr:rowOff>
+      <xdr:rowOff>285840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>405360</xdr:colOff>
+      <xdr:colOff>432360</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>295200</xdr:rowOff>
+      <xdr:rowOff>286200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2343,7 +2355,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8216640" y="5040000"/>
+          <a:off x="8243640" y="5031000"/>
           <a:ext cx="360" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -2369,15 +2381,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>900000</xdr:colOff>
+      <xdr:colOff>927000</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>161280</xdr:rowOff>
+      <xdr:rowOff>152280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>79200</xdr:colOff>
+      <xdr:colOff>105840</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>161640</xdr:rowOff>
+      <xdr:rowOff>152640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2386,8 +2398,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4964400" y="5258880"/>
-          <a:ext cx="5390280" cy="360"/>
+          <a:off x="4991400" y="5249880"/>
+          <a:ext cx="5389920" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2409,15 +2421,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1059480</xdr:colOff>
+      <xdr:colOff>1086480</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>65520</xdr:rowOff>
+      <xdr:rowOff>56520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>706680</xdr:colOff>
+      <xdr:colOff>733320</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>32040</xdr:rowOff>
+      <xdr:rowOff>22680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2430,8 +2442,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7537680" y="65520"/>
-          <a:ext cx="3444480" cy="823680"/>
+          <a:off x="7564680" y="56520"/>
+          <a:ext cx="3444120" cy="823320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2451,15 +2463,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>785880</xdr:colOff>
+      <xdr:colOff>812880</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>39600</xdr:rowOff>
+      <xdr:rowOff>30600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>312120</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>6120</xdr:rowOff>
+      <xdr:colOff>338760</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>853920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2472,8 +2484,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10439640" y="39600"/>
-          <a:ext cx="3489840" cy="823680"/>
+          <a:off x="10466640" y="30600"/>
+          <a:ext cx="3489480" cy="823320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2493,15 +2505,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1043280</xdr:colOff>
+      <xdr:colOff>1070280</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>397440</xdr:colOff>
+      <xdr:colOff>424080</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>823680</xdr:rowOff>
+      <xdr:rowOff>823320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2514,8 +2526,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8528400" y="0"/>
-          <a:ext cx="3546000" cy="823680"/>
+          <a:off x="8555400" y="0"/>
+          <a:ext cx="3545640" cy="823320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2535,15 +2547,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1632600</xdr:colOff>
+      <xdr:colOff>1659600</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1808280</xdr:colOff>
+      <xdr:colOff>1834920</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>823680</xdr:rowOff>
+      <xdr:rowOff>823320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2556,8 +2568,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15007320" y="0"/>
-          <a:ext cx="3274560" cy="823680"/>
+          <a:off x="15034320" y="0"/>
+          <a:ext cx="3274200" cy="823320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2579,8 +2591,8 @@
   </sheetPr>
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2875,8 +2887,8 @@
   </sheetPr>
   <dimension ref="A1:G65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2945,10 +2957,10 @@
       <c r="E5" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="F5" s="37"/>
+      <c r="F5" s="36"/>
     </row>
     <row r="6" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="38"/>
+      <c r="A6" s="37"/>
       <c r="B6" s="33" t="s">
         <v>6</v>
       </c>
@@ -2958,13 +2970,13 @@
       <c r="D6" s="35" t="n">
         <v>3318039095</v>
       </c>
-      <c r="E6" s="39" t="s">
+      <c r="E6" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="F6" s="39"/>
+      <c r="F6" s="36"/>
     </row>
     <row r="7" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="38"/>
+      <c r="A7" s="37"/>
       <c r="B7" s="33" t="s">
         <v>6</v>
       </c>
@@ -2974,13 +2986,13 @@
       <c r="D7" s="35" t="n">
         <v>3318039095</v>
       </c>
-      <c r="E7" s="39" t="s">
+      <c r="E7" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="39"/>
+      <c r="F7" s="36"/>
     </row>
     <row r="8" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="38"/>
+      <c r="A8" s="37"/>
       <c r="B8" s="33" t="s">
         <v>45</v>
       </c>
@@ -2990,13 +3002,13 @@
       <c r="D8" s="35" t="n">
         <v>3319638873</v>
       </c>
-      <c r="E8" s="40" t="s">
+      <c r="E8" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="F8" s="40"/>
+      <c r="F8" s="38"/>
     </row>
     <row r="9" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="38"/>
+      <c r="A9" s="37"/>
       <c r="B9" s="33" t="s">
         <v>48</v>
       </c>
@@ -3006,13 +3018,13 @@
       <c r="D9" s="35" t="n">
         <v>3312430761</v>
       </c>
-      <c r="E9" s="40" t="s">
+      <c r="E9" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="40"/>
+      <c r="F9" s="39"/>
     </row>
     <row r="10" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="38"/>
+      <c r="A10" s="37"/>
       <c r="B10" s="33" t="s">
         <v>51</v>
       </c>
@@ -3022,13 +3034,13 @@
       <c r="D10" s="35" t="n">
         <v>3310739239</v>
       </c>
-      <c r="E10" s="40" t="s">
+      <c r="E10" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="F10" s="40"/>
+      <c r="F10" s="39"/>
     </row>
     <row r="11" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="38"/>
+      <c r="A11" s="37"/>
       <c r="B11" s="33" t="s">
         <v>51</v>
       </c>
@@ -3038,18 +3050,18 @@
       <c r="D11" s="35" t="n">
         <v>3310739239</v>
       </c>
-      <c r="E11" s="40" t="s">
+      <c r="E11" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="F11" s="40"/>
+      <c r="F11" s="39"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="41"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="42"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
+      <c r="A12" s="40"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
     </row>
     <row r="13" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B13" s="29" t="s">
@@ -3057,54 +3069,54 @@
       </c>
     </row>
     <row r="14" s="30" customFormat="true" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="44" t="s">
+      <c r="B14" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="C14" s="44" t="s">
+      <c r="C14" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="D14" s="44" t="s">
+      <c r="D14" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="E14" s="44" t="s">
+      <c r="E14" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="G14" s="45"/>
+      <c r="G14" s="44"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="46" t="s">
+      <c r="B15" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="C15" s="47"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="48"/>
-      <c r="G15" s="49"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="47"/>
+      <c r="G15" s="48"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="46"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="47"/>
-      <c r="E16" s="48"/>
+      <c r="B16" s="45"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="47"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="46"/>
-      <c r="C17" s="47"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="48"/>
+      <c r="B17" s="45"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="47"/>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="46"/>
-      <c r="C18" s="47"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="48"/>
+      <c r="B18" s="45"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="47"/>
     </row>
     <row r="19" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C19" s="50"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="50"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
     </row>
     <row r="20" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="51" t="s">
+      <c r="B20" s="50" t="s">
         <v>61</v>
       </c>
     </row>
@@ -3125,59 +3137,59 @@
       <c r="G21" s="32"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B22" s="52" t="s">
+      <c r="B22" s="51" t="s">
         <v>62</v>
       </c>
-      <c r="C22" s="53" t="s">
+      <c r="C22" s="52" t="s">
         <v>63</v>
       </c>
       <c r="D22" s="35"/>
-      <c r="E22" s="54" t="s">
+      <c r="E22" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="F22" s="54"/>
+      <c r="F22" s="53"/>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="52"/>
-      <c r="C23" s="53"/>
+      <c r="B23" s="51"/>
+      <c r="C23" s="52"/>
       <c r="D23" s="35"/>
-      <c r="E23" s="54"/>
-      <c r="F23" s="54"/>
+      <c r="E23" s="53"/>
+      <c r="F23" s="53"/>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="52"/>
-      <c r="C24" s="53"/>
+      <c r="B24" s="51"/>
+      <c r="C24" s="52"/>
       <c r="D24" s="35"/>
-      <c r="E24" s="54"/>
-      <c r="F24" s="54"/>
+      <c r="E24" s="53"/>
+      <c r="F24" s="53"/>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="52"/>
-      <c r="C25" s="53"/>
+      <c r="B25" s="51"/>
+      <c r="C25" s="52"/>
       <c r="D25" s="35"/>
-      <c r="E25" s="54"/>
-      <c r="F25" s="54"/>
+      <c r="E25" s="53"/>
+      <c r="F25" s="53"/>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="52"/>
-      <c r="C26" s="53"/>
+      <c r="B26" s="51"/>
+      <c r="C26" s="52"/>
       <c r="D26" s="35"/>
-      <c r="E26" s="54"/>
-      <c r="F26" s="54"/>
+      <c r="E26" s="53"/>
+      <c r="F26" s="53"/>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="52"/>
-      <c r="C27" s="53"/>
+      <c r="B27" s="51"/>
+      <c r="C27" s="52"/>
       <c r="D27" s="35"/>
-      <c r="E27" s="54"/>
-      <c r="F27" s="54"/>
+      <c r="E27" s="53"/>
+      <c r="F27" s="53"/>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="52"/>
-      <c r="C28" s="53"/>
+      <c r="B28" s="51"/>
+      <c r="C28" s="52"/>
       <c r="D28" s="35"/>
-      <c r="E28" s="54"/>
-      <c r="F28" s="54"/>
+      <c r="E28" s="53"/>
+      <c r="F28" s="53"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3189,8 +3201,9 @@
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
     <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
@@ -3221,10 +3234,7 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E5" r:id="rId1" display="anayelizp@bisoltec.com.mx"/>
-    <hyperlink ref="E6" r:id="rId2" display="zepeda.roque32@gmail.com"/>
-    <hyperlink ref="E7" r:id="rId3" display="zepeda.roque32@gmail.com"/>
-    <hyperlink ref="E22" r:id="rId4" display="rpulido@qualtop.com"/>
+    <hyperlink ref="E22" r:id="rId1" display="rpulido@qualtop.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3233,7 +3243,7 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId5"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3244,8 +3254,8 @@
   </sheetPr>
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3306,249 +3316,249 @@
   <sheetData>
     <row r="1" customFormat="false" ht="67.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="55"/>
+      <c r="A2" s="54"/>
     </row>
     <row r="3" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="56"/>
-      <c r="B3" s="57" t="s">
+      <c r="A3" s="55"/>
+      <c r="B3" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-    </row>
-    <row r="4" s="63" customFormat="true" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="59"/>
-      <c r="B4" s="60" t="s">
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+    </row>
+    <row r="4" s="62" customFormat="true" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="58"/>
+      <c r="B4" s="59" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="61" t="s">
+      <c r="C4" s="60" t="s">
         <v>67</v>
       </c>
-      <c r="D4" s="61" t="s">
+      <c r="D4" s="60" t="s">
         <v>68</v>
       </c>
-      <c r="E4" s="61" t="s">
+      <c r="E4" s="60" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="61" t="s">
+      <c r="F4" s="60" t="s">
         <v>70</v>
       </c>
-      <c r="G4" s="62" t="s">
+      <c r="G4" s="61" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="64" t="s">
+      <c r="B5" s="63" t="s">
         <v>72</v>
       </c>
-      <c r="C5" s="65" t="s">
+      <c r="C5" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="66" t="s">
+      <c r="D5" s="65" t="s">
         <v>73</v>
       </c>
-      <c r="E5" s="65" t="s">
+      <c r="E5" s="64" t="s">
         <v>74</v>
       </c>
-      <c r="F5" s="65" t="s">
+      <c r="F5" s="64" t="s">
         <v>75</v>
       </c>
-      <c r="G5" s="67"/>
+      <c r="G5" s="66"/>
     </row>
     <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="64" t="s">
+      <c r="B6" s="63" t="s">
         <v>76</v>
       </c>
-      <c r="C6" s="65" t="s">
+      <c r="C6" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="66" t="s">
+      <c r="D6" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="65" t="s">
+      <c r="E6" s="64" t="s">
         <v>77</v>
       </c>
-      <c r="F6" s="65" t="s">
+      <c r="F6" s="64" t="s">
         <v>78</v>
       </c>
-      <c r="G6" s="67"/>
-      <c r="L6" s="68"/>
+      <c r="G6" s="66"/>
+      <c r="L6" s="67"/>
     </row>
     <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="64" t="s">
+      <c r="B7" s="63" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="65" t="s">
+      <c r="C7" s="64" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="66" t="s">
+      <c r="D7" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="65" t="s">
+      <c r="E7" s="64" t="s">
         <v>80</v>
       </c>
-      <c r="F7" s="65" t="s">
+      <c r="F7" s="64" t="s">
         <v>75</v>
       </c>
-      <c r="G7" s="67"/>
-      <c r="L7" s="68"/>
+      <c r="G7" s="66"/>
+      <c r="L7" s="67"/>
     </row>
     <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="64"/>
-      <c r="C8" s="65"/>
-      <c r="D8" s="66"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="65"/>
-      <c r="G8" s="67"/>
-      <c r="L8" s="68"/>
+      <c r="B8" s="63"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="66"/>
+      <c r="L8" s="67"/>
     </row>
     <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="64"/>
-      <c r="C9" s="65"/>
-      <c r="D9" s="66"/>
-      <c r="E9" s="65"/>
-      <c r="F9" s="65"/>
-      <c r="G9" s="67"/>
-      <c r="L9" s="68"/>
+      <c r="B9" s="63"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="66"/>
+      <c r="L9" s="67"/>
     </row>
     <row r="10" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="64"/>
-      <c r="C10" s="65"/>
-      <c r="D10" s="66"/>
-      <c r="E10" s="65"/>
-      <c r="F10" s="65"/>
-      <c r="G10" s="67"/>
-      <c r="L10" s="68"/>
+      <c r="B10" s="63"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="64"/>
+      <c r="F10" s="64"/>
+      <c r="G10" s="66"/>
+      <c r="L10" s="67"/>
     </row>
     <row r="11" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="64"/>
-      <c r="C11" s="65"/>
-      <c r="D11" s="66"/>
-      <c r="E11" s="65"/>
-      <c r="F11" s="65"/>
-      <c r="G11" s="67"/>
-      <c r="L11" s="68"/>
+      <c r="B11" s="63"/>
+      <c r="C11" s="64"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="66"/>
+      <c r="L11" s="67"/>
     </row>
     <row r="12" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="64"/>
-      <c r="C12" s="65"/>
-      <c r="D12" s="66"/>
-      <c r="E12" s="65"/>
-      <c r="F12" s="65"/>
-      <c r="G12" s="67"/>
-      <c r="L12" s="68"/>
+      <c r="B12" s="63"/>
+      <c r="C12" s="64"/>
+      <c r="D12" s="65"/>
+      <c r="E12" s="64"/>
+      <c r="F12" s="64"/>
+      <c r="G12" s="66"/>
+      <c r="L12" s="67"/>
     </row>
     <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="64"/>
-      <c r="C13" s="65"/>
-      <c r="D13" s="66"/>
-      <c r="E13" s="65"/>
-      <c r="F13" s="65"/>
-      <c r="G13" s="67"/>
-      <c r="L13" s="68"/>
+      <c r="B13" s="63"/>
+      <c r="C13" s="64"/>
+      <c r="D13" s="65"/>
+      <c r="E13" s="64"/>
+      <c r="F13" s="64"/>
+      <c r="G13" s="66"/>
+      <c r="L13" s="67"/>
     </row>
     <row r="14" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="64"/>
-      <c r="C14" s="65"/>
-      <c r="D14" s="66"/>
-      <c r="E14" s="65"/>
-      <c r="F14" s="65"/>
-      <c r="G14" s="67"/>
-      <c r="L14" s="68"/>
+      <c r="B14" s="63"/>
+      <c r="C14" s="64"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="64"/>
+      <c r="F14" s="64"/>
+      <c r="G14" s="66"/>
+      <c r="L14" s="67"/>
     </row>
     <row r="15" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="64"/>
-      <c r="C15" s="65"/>
-      <c r="D15" s="66"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="65"/>
-      <c r="G15" s="67"/>
+      <c r="B15" s="63"/>
+      <c r="C15" s="64"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="64"/>
+      <c r="F15" s="64"/>
+      <c r="G15" s="66"/>
     </row>
     <row r="16" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="64"/>
-      <c r="C16" s="65"/>
-      <c r="D16" s="66"/>
-      <c r="E16" s="65"/>
-      <c r="F16" s="65"/>
-      <c r="G16" s="67"/>
-      <c r="L16" s="68"/>
+      <c r="B16" s="63"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="65"/>
+      <c r="E16" s="64"/>
+      <c r="F16" s="64"/>
+      <c r="G16" s="66"/>
+      <c r="L16" s="67"/>
     </row>
     <row r="17" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="64"/>
-      <c r="C17" s="65"/>
-      <c r="D17" s="66"/>
-      <c r="E17" s="65"/>
-      <c r="F17" s="65"/>
-      <c r="G17" s="67"/>
-      <c r="L17" s="68"/>
+      <c r="B17" s="63"/>
+      <c r="C17" s="64"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="64"/>
+      <c r="F17" s="64"/>
+      <c r="G17" s="66"/>
+      <c r="L17" s="67"/>
     </row>
     <row r="18" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="64"/>
-      <c r="C18" s="65"/>
-      <c r="D18" s="66"/>
-      <c r="E18" s="65"/>
-      <c r="F18" s="65"/>
-      <c r="G18" s="67"/>
-      <c r="L18" s="68"/>
+      <c r="B18" s="63"/>
+      <c r="C18" s="64"/>
+      <c r="D18" s="65"/>
+      <c r="E18" s="64"/>
+      <c r="F18" s="64"/>
+      <c r="G18" s="66"/>
+      <c r="L18" s="67"/>
     </row>
     <row r="19" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="64"/>
-      <c r="C19" s="65"/>
-      <c r="D19" s="66"/>
-      <c r="E19" s="65"/>
-      <c r="F19" s="65"/>
-      <c r="G19" s="67"/>
+      <c r="B19" s="63"/>
+      <c r="C19" s="64"/>
+      <c r="D19" s="65"/>
+      <c r="E19" s="64"/>
+      <c r="F19" s="64"/>
+      <c r="G19" s="66"/>
     </row>
     <row r="20" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="64"/>
-      <c r="C20" s="65"/>
-      <c r="D20" s="66"/>
-      <c r="E20" s="65"/>
-      <c r="F20" s="65"/>
-      <c r="G20" s="67"/>
+      <c r="B20" s="63"/>
+      <c r="C20" s="64"/>
+      <c r="D20" s="65"/>
+      <c r="E20" s="64"/>
+      <c r="F20" s="64"/>
+      <c r="G20" s="66"/>
     </row>
     <row r="21" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="64"/>
-      <c r="C21" s="65"/>
-      <c r="D21" s="66"/>
-      <c r="E21" s="65"/>
-      <c r="F21" s="65"/>
-      <c r="G21" s="67"/>
+      <c r="B21" s="63"/>
+      <c r="C21" s="64"/>
+      <c r="D21" s="65"/>
+      <c r="E21" s="64"/>
+      <c r="F21" s="64"/>
+      <c r="G21" s="66"/>
     </row>
     <row r="22" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="64"/>
-      <c r="C22" s="65"/>
-      <c r="D22" s="66"/>
-      <c r="E22" s="65"/>
-      <c r="F22" s="65"/>
-      <c r="G22" s="67"/>
+      <c r="B22" s="63"/>
+      <c r="C22" s="64"/>
+      <c r="D22" s="65"/>
+      <c r="E22" s="64"/>
+      <c r="F22" s="64"/>
+      <c r="G22" s="66"/>
     </row>
     <row r="23" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="64"/>
-      <c r="C23" s="65"/>
-      <c r="D23" s="66"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="65"/>
-      <c r="G23" s="67"/>
+      <c r="B23" s="63"/>
+      <c r="C23" s="64"/>
+      <c r="D23" s="65"/>
+      <c r="E23" s="64"/>
+      <c r="F23" s="64"/>
+      <c r="G23" s="66"/>
     </row>
     <row r="24" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="64"/>
-      <c r="C24" s="65"/>
-      <c r="D24" s="66"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="65"/>
-      <c r="G24" s="67"/>
+      <c r="B24" s="63"/>
+      <c r="C24" s="64"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="64"/>
+      <c r="F24" s="64"/>
+      <c r="G24" s="66"/>
     </row>
     <row r="25" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="64"/>
-      <c r="C25" s="65"/>
-      <c r="D25" s="66"/>
-      <c r="E25" s="65"/>
-      <c r="F25" s="65"/>
-      <c r="G25" s="67"/>
+      <c r="B25" s="63"/>
+      <c r="C25" s="64"/>
+      <c r="D25" s="65"/>
+      <c r="E25" s="64"/>
+      <c r="F25" s="64"/>
+      <c r="G25" s="66"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -3576,8 +3586,8 @@
   </sheetPr>
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3594,206 +3604,206 @@
     <row r="1" customFormat="false" ht="67.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="69" t="s">
+      <c r="A3" s="68" t="s">
         <v>81</v>
       </c>
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
     </row>
     <row r="4" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="B4" s="72" t="s">
+      <c r="B4" s="71" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="72" t="s">
+      <c r="C4" s="71" t="s">
         <v>84</v>
       </c>
-      <c r="D4" s="72" t="s">
+      <c r="D4" s="71" t="s">
         <v>85</v>
       </c>
-      <c r="E4" s="72" t="s">
+      <c r="E4" s="71" t="s">
         <v>86</v>
       </c>
-      <c r="F4" s="72" t="s">
+      <c r="F4" s="71" t="s">
         <v>87</v>
       </c>
-      <c r="G4" s="73" t="s">
+      <c r="G4" s="72" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="74" t="s">
+      <c r="A5" s="73" t="s">
         <v>89</v>
       </c>
-      <c r="B5" s="75" t="s">
+      <c r="B5" s="74" t="s">
         <v>90</v>
       </c>
-      <c r="C5" s="75"/>
-      <c r="D5" s="75" t="n">
+      <c r="C5" s="74"/>
+      <c r="D5" s="74" t="n">
         <v>5</v>
       </c>
-      <c r="E5" s="76" t="n">
+      <c r="E5" s="75" t="n">
         <v>42443</v>
       </c>
-      <c r="F5" s="76" t="n">
+      <c r="F5" s="75" t="n">
         <v>42443</v>
       </c>
-      <c r="G5" s="77"/>
-      <c r="J5" s="78" t="s">
+      <c r="G5" s="76"/>
+      <c r="J5" s="77" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="74" t="s">
+      <c r="A6" s="73" t="s">
         <v>92</v>
       </c>
-      <c r="B6" s="75" t="s">
+      <c r="B6" s="74" t="s">
         <v>93</v>
       </c>
-      <c r="C6" s="75"/>
-      <c r="D6" s="75" t="n">
+      <c r="C6" s="74"/>
+      <c r="D6" s="74" t="n">
         <v>5</v>
       </c>
-      <c r="E6" s="76" t="n">
+      <c r="E6" s="75" t="n">
         <v>42443</v>
       </c>
-      <c r="F6" s="76" t="n">
+      <c r="F6" s="75" t="n">
         <v>42443</v>
       </c>
-      <c r="G6" s="77"/>
-      <c r="J6" s="78" t="s">
+      <c r="G6" s="76"/>
+      <c r="J6" s="77" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="74" t="s">
+      <c r="A7" s="73" t="s">
         <v>94</v>
       </c>
-      <c r="B7" s="75" t="s">
+      <c r="B7" s="74" t="s">
         <v>93</v>
       </c>
-      <c r="C7" s="75"/>
-      <c r="D7" s="75" t="n">
+      <c r="C7" s="74"/>
+      <c r="D7" s="74" t="n">
         <v>5</v>
       </c>
-      <c r="E7" s="76" t="n">
+      <c r="E7" s="75" t="n">
         <v>42443</v>
       </c>
-      <c r="F7" s="76" t="n">
+      <c r="F7" s="75" t="n">
         <v>42443</v>
       </c>
-      <c r="G7" s="77"/>
-      <c r="J7" s="78" t="s">
+      <c r="G7" s="76"/>
+      <c r="J7" s="77" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="74" t="s">
+      <c r="A8" s="73" t="s">
         <v>96</v>
       </c>
-      <c r="B8" s="75" t="s">
+      <c r="B8" s="74" t="s">
         <v>93</v>
       </c>
-      <c r="C8" s="75"/>
-      <c r="D8" s="75" t="n">
+      <c r="C8" s="74"/>
+      <c r="D8" s="74" t="n">
         <v>2</v>
       </c>
-      <c r="E8" s="76" t="n">
+      <c r="E8" s="75" t="n">
         <v>42443</v>
       </c>
-      <c r="F8" s="76" t="n">
+      <c r="F8" s="75" t="n">
         <v>42443</v>
       </c>
-      <c r="G8" s="77"/>
-      <c r="J8" s="78"/>
+      <c r="G8" s="76"/>
+      <c r="J8" s="77"/>
     </row>
     <row r="9" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="74" t="s">
+      <c r="A9" s="73" t="s">
         <v>97</v>
       </c>
-      <c r="B9" s="75" t="s">
+      <c r="B9" s="74" t="s">
         <v>95</v>
       </c>
-      <c r="C9" s="75"/>
-      <c r="D9" s="75" t="n">
+      <c r="C9" s="74"/>
+      <c r="D9" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="E9" s="76" t="n">
+      <c r="E9" s="75" t="n">
         <v>42443</v>
       </c>
-      <c r="F9" s="76" t="n">
+      <c r="F9" s="75" t="n">
         <v>42443</v>
       </c>
-      <c r="G9" s="77"/>
+      <c r="G9" s="76"/>
     </row>
     <row r="10" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="74"/>
-      <c r="B10" s="75"/>
-      <c r="C10" s="75"/>
-      <c r="D10" s="75"/>
-      <c r="E10" s="75"/>
-      <c r="F10" s="75"/>
-      <c r="G10" s="77"/>
+      <c r="A10" s="73"/>
+      <c r="B10" s="74"/>
+      <c r="C10" s="74"/>
+      <c r="D10" s="74"/>
+      <c r="E10" s="74"/>
+      <c r="F10" s="74"/>
+      <c r="G10" s="76"/>
     </row>
     <row r="11" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="74"/>
-      <c r="B11" s="75"/>
-      <c r="C11" s="75"/>
-      <c r="D11" s="75"/>
-      <c r="E11" s="75"/>
-      <c r="F11" s="75"/>
-      <c r="G11" s="77"/>
+      <c r="A11" s="73"/>
+      <c r="B11" s="74"/>
+      <c r="C11" s="74"/>
+      <c r="D11" s="74"/>
+      <c r="E11" s="74"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="76"/>
     </row>
     <row r="12" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="74"/>
-      <c r="B12" s="75"/>
-      <c r="C12" s="75"/>
-      <c r="D12" s="75"/>
-      <c r="E12" s="75"/>
-      <c r="F12" s="75"/>
-      <c r="G12" s="77"/>
+      <c r="A12" s="73"/>
+      <c r="B12" s="74"/>
+      <c r="C12" s="74"/>
+      <c r="D12" s="74"/>
+      <c r="E12" s="74"/>
+      <c r="F12" s="74"/>
+      <c r="G12" s="76"/>
     </row>
     <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="74"/>
-      <c r="B13" s="75"/>
-      <c r="C13" s="75"/>
-      <c r="D13" s="75"/>
-      <c r="E13" s="75"/>
-      <c r="F13" s="75"/>
-      <c r="G13" s="77"/>
+      <c r="A13" s="73"/>
+      <c r="B13" s="74"/>
+      <c r="C13" s="74"/>
+      <c r="D13" s="74"/>
+      <c r="E13" s="74"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="76"/>
     </row>
     <row r="14" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="74"/>
-      <c r="B14" s="75"/>
-      <c r="C14" s="75"/>
-      <c r="D14" s="75"/>
-      <c r="E14" s="75"/>
-      <c r="F14" s="75"/>
-      <c r="G14" s="77"/>
+      <c r="A14" s="73"/>
+      <c r="B14" s="74"/>
+      <c r="C14" s="74"/>
+      <c r="D14" s="74"/>
+      <c r="E14" s="74"/>
+      <c r="F14" s="74"/>
+      <c r="G14" s="76"/>
     </row>
     <row r="15" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="74"/>
-      <c r="B15" s="75"/>
-      <c r="C15" s="75"/>
-      <c r="D15" s="75"/>
-      <c r="E15" s="75"/>
-      <c r="F15" s="75"/>
-      <c r="G15" s="77"/>
+      <c r="A15" s="73"/>
+      <c r="B15" s="74"/>
+      <c r="C15" s="74"/>
+      <c r="D15" s="74"/>
+      <c r="E15" s="74"/>
+      <c r="F15" s="74"/>
+      <c r="G15" s="76"/>
     </row>
     <row r="16" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="74"/>
-      <c r="B16" s="75"/>
-      <c r="C16" s="75"/>
-      <c r="D16" s="75"/>
-      <c r="E16" s="75"/>
-      <c r="F16" s="75"/>
-      <c r="G16" s="77"/>
+      <c r="A16" s="73"/>
+      <c r="B16" s="74"/>
+      <c r="C16" s="74"/>
+      <c r="D16" s="74"/>
+      <c r="E16" s="74"/>
+      <c r="F16" s="74"/>
+      <c r="G16" s="76"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -3825,8 +3835,8 @@
   </sheetPr>
   <dimension ref="A1:IZ20"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G7" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J10" activeCellId="0" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -3854,1007 +3864,1019 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="68.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
     </row>
     <row r="2" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="80"/>
-      <c r="B2" s="81"/>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="83"/>
-      <c r="IQ2" s="84" t="s">
+      <c r="A2" s="79"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="82"/>
+      <c r="IQ2" s="83" t="s">
         <v>98</v>
       </c>
-      <c r="IR2" s="84"/>
-      <c r="IS2" s="84"/>
-      <c r="IT2" s="84"/>
-      <c r="IU2" s="84"/>
-      <c r="IV2" s="84"/>
-      <c r="IW2" s="84"/>
-      <c r="IX2" s="84"/>
-      <c r="IY2" s="84"/>
-      <c r="IZ2" s="84"/>
+      <c r="IR2" s="83"/>
+      <c r="IS2" s="83"/>
+      <c r="IT2" s="83"/>
+      <c r="IU2" s="83"/>
+      <c r="IV2" s="83"/>
+      <c r="IW2" s="83"/>
+      <c r="IX2" s="83"/>
+      <c r="IY2" s="83"/>
+      <c r="IZ2" s="83"/>
     </row>
     <row r="3" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="85" t="s">
+      <c r="A3" s="84" t="s">
         <v>99</v>
       </c>
-      <c r="B3" s="86"/>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
-      <c r="H3" s="88"/>
-      <c r="I3" s="88"/>
-      <c r="J3" s="88"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="R3" s="90"/>
-      <c r="AD3" s="91" t="s">
+      <c r="B3" s="85"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="L3" s="88"/>
+      <c r="M3" s="88"/>
+      <c r="R3" s="89"/>
+      <c r="AD3" s="90" t="s">
         <v>100</v>
       </c>
-      <c r="AE3" s="91" t="s">
+      <c r="AE3" s="90" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="92" t="s">
+      <c r="A4" s="91" t="s">
         <v>102</v>
       </c>
-      <c r="B4" s="92" t="s">
+      <c r="B4" s="91" t="s">
         <v>103</v>
       </c>
-      <c r="C4" s="93" t="s">
+      <c r="C4" s="92" t="s">
         <v>104</v>
       </c>
-      <c r="D4" s="93" t="s">
+      <c r="D4" s="92" t="s">
         <v>105</v>
       </c>
-      <c r="E4" s="93" t="s">
+      <c r="E4" s="92" t="s">
         <v>106</v>
       </c>
-      <c r="F4" s="93" t="s">
+      <c r="F4" s="92" t="s">
         <v>107</v>
       </c>
-      <c r="G4" s="93" t="s">
+      <c r="G4" s="92" t="s">
         <v>108</v>
       </c>
-      <c r="H4" s="93" t="s">
+      <c r="H4" s="92" t="s">
         <v>67</v>
       </c>
-      <c r="I4" s="93" t="s">
+      <c r="I4" s="92" t="s">
         <v>109</v>
       </c>
-      <c r="J4" s="93" t="s">
+      <c r="J4" s="92" t="s">
         <v>110</v>
       </c>
-      <c r="L4" s="94" t="s">
+      <c r="L4" s="93" t="s">
         <v>105</v>
       </c>
-      <c r="M4" s="95" t="n">
+      <c r="M4" s="94" t="n">
         <v>5</v>
       </c>
-      <c r="N4" s="96" t="n">
+      <c r="N4" s="95" t="n">
         <v>5</v>
       </c>
-      <c r="O4" s="97" t="n">
+      <c r="O4" s="96" t="n">
         <v>10</v>
       </c>
-      <c r="P4" s="98" t="n">
+      <c r="P4" s="97" t="n">
         <v>15</v>
       </c>
-      <c r="Q4" s="99" t="n">
+      <c r="Q4" s="98" t="n">
         <v>20</v>
       </c>
-      <c r="R4" s="100" t="n">
+      <c r="R4" s="99" t="n">
         <v>25</v>
       </c>
-      <c r="S4" s="101"/>
-      <c r="T4" s="102" t="s">
+      <c r="S4" s="100"/>
+      <c r="T4" s="101" t="s">
         <v>111</v>
       </c>
-      <c r="U4" s="102"/>
-      <c r="AD4" s="91" t="s">
+      <c r="U4" s="101"/>
+      <c r="AD4" s="90" t="s">
         <v>100</v>
       </c>
-      <c r="AE4" s="91" t="s">
+      <c r="AE4" s="90" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="45.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="103" t="n">
+      <c r="A5" s="102" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="104" t="s">
+      <c r="B5" s="103" t="s">
         <v>112</v>
       </c>
-      <c r="C5" s="105" t="n">
+      <c r="C5" s="104" t="n">
         <v>3</v>
       </c>
-      <c r="D5" s="105" t="n">
+      <c r="D5" s="104" t="n">
         <v>3</v>
       </c>
-      <c r="E5" s="105" t="n">
+      <c r="E5" s="104" t="n">
         <f aca="false">PRODUCT(C5:D5)</f>
         <v>9</v>
       </c>
-      <c r="F5" s="104" t="s">
+      <c r="F5" s="103" t="s">
         <v>113</v>
       </c>
-      <c r="G5" s="104" t="s">
+      <c r="G5" s="103" t="s">
         <v>114</v>
       </c>
-      <c r="H5" s="105" t="s">
+      <c r="H5" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="105" t="s">
+      <c r="I5" s="104" t="s">
         <v>115</v>
       </c>
-      <c r="J5" s="106"/>
-      <c r="K5" s="107"/>
-      <c r="L5" s="94"/>
-      <c r="M5" s="95" t="n">
+      <c r="J5" s="105" t="s">
+        <v>116</v>
+      </c>
+      <c r="K5" s="106"/>
+      <c r="L5" s="93"/>
+      <c r="M5" s="94" t="n">
         <v>4</v>
       </c>
-      <c r="N5" s="108" t="n">
+      <c r="N5" s="107" t="n">
         <v>4</v>
       </c>
-      <c r="O5" s="109" t="n">
+      <c r="O5" s="108" t="n">
         <v>8</v>
       </c>
-      <c r="P5" s="110" t="n">
+      <c r="P5" s="109" t="n">
         <v>12</v>
       </c>
-      <c r="Q5" s="100" t="n">
+      <c r="Q5" s="99" t="n">
         <v>16</v>
       </c>
-      <c r="R5" s="100" t="n">
+      <c r="R5" s="99" t="n">
         <v>20</v>
       </c>
-      <c r="S5" s="101"/>
-      <c r="T5" s="111" t="s">
-        <v>116</v>
-      </c>
-      <c r="U5" s="112" t="s">
+      <c r="S5" s="100"/>
+      <c r="T5" s="110" t="s">
+        <v>117</v>
+      </c>
+      <c r="U5" s="111" t="s">
         <v>104</v>
       </c>
-      <c r="IR5" s="113" t="s">
+      <c r="IR5" s="112" t="s">
         <v>105</v>
       </c>
-      <c r="IS5" s="114" t="s">
-        <v>117</v>
-      </c>
-      <c r="IT5" s="43" t="n">
+      <c r="IS5" s="113" t="s">
+        <v>118</v>
+      </c>
+      <c r="IT5" s="42" t="n">
         <v>0.9</v>
       </c>
-      <c r="IU5" s="115" t="n">
+      <c r="IU5" s="114" t="n">
         <f aca="false">(IU10*IT5)</f>
         <v>0.9</v>
       </c>
-      <c r="IV5" s="115" t="n">
+      <c r="IV5" s="114" t="n">
         <f aca="false">(IV10*IT5)</f>
         <v>1.8</v>
       </c>
-      <c r="IW5" s="116" t="n">
+      <c r="IW5" s="115" t="n">
         <f aca="false">(IW10*IT5)</f>
         <v>2.7</v>
       </c>
-      <c r="IX5" s="89" t="n">
+      <c r="IX5" s="88" t="n">
         <f aca="false">(IX10*IT5)</f>
         <v>3.6</v>
       </c>
-      <c r="IY5" s="117" t="n">
+      <c r="IY5" s="116" t="n">
         <f aca="false">(IY10*IT5)</f>
         <v>4.5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="47.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="103" t="n">
+      <c r="A6" s="102" t="n">
         <f aca="false">A5+1</f>
         <v>2</v>
       </c>
-      <c r="B6" s="104" t="s">
-        <v>118</v>
-      </c>
-      <c r="C6" s="105" t="n">
+      <c r="B6" s="103" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6" s="104" t="n">
         <v>4</v>
       </c>
-      <c r="D6" s="105" t="n">
+      <c r="D6" s="104" t="n">
         <v>3</v>
       </c>
-      <c r="E6" s="105" t="n">
+      <c r="E6" s="104" t="n">
         <f aca="false">PRODUCT(C6:D6)</f>
         <v>12</v>
       </c>
-      <c r="F6" s="104" t="s">
-        <v>119</v>
-      </c>
-      <c r="G6" s="104" t="s">
+      <c r="F6" s="103" t="s">
         <v>120</v>
       </c>
-      <c r="H6" s="105" t="s">
+      <c r="G6" s="103" t="s">
+        <v>121</v>
+      </c>
+      <c r="H6" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="105" t="s">
+      <c r="I6" s="104" t="s">
         <v>115</v>
       </c>
-      <c r="J6" s="106"/>
-      <c r="K6" s="107"/>
-      <c r="L6" s="94"/>
-      <c r="M6" s="95" t="n">
+      <c r="J6" s="105" t="s">
+        <v>116</v>
+      </c>
+      <c r="K6" s="106"/>
+      <c r="L6" s="93"/>
+      <c r="M6" s="94" t="n">
         <v>3</v>
       </c>
-      <c r="N6" s="118" t="n">
+      <c r="N6" s="117" t="n">
         <v>3</v>
       </c>
-      <c r="O6" s="119" t="n">
+      <c r="O6" s="118" t="n">
         <v>6</v>
       </c>
-      <c r="P6" s="97" t="n">
+      <c r="P6" s="96" t="n">
         <v>9</v>
       </c>
-      <c r="Q6" s="100" t="n">
+      <c r="Q6" s="99" t="n">
         <v>12</v>
       </c>
-      <c r="R6" s="100" t="n">
+      <c r="R6" s="99" t="n">
         <v>15</v>
       </c>
-      <c r="S6" s="101"/>
-      <c r="T6" s="120" t="n">
+      <c r="S6" s="100"/>
+      <c r="T6" s="119" t="n">
         <v>1</v>
       </c>
-      <c r="U6" s="121" t="s">
-        <v>121</v>
-      </c>
-      <c r="IR6" s="113"/>
-      <c r="IS6" s="114" t="s">
+      <c r="U6" s="120" t="s">
         <v>122</v>
       </c>
-      <c r="IT6" s="43" t="n">
+      <c r="IR6" s="112"/>
+      <c r="IS6" s="113" t="s">
+        <v>123</v>
+      </c>
+      <c r="IT6" s="42" t="n">
         <v>0.7</v>
       </c>
-      <c r="IU6" s="122" t="n">
+      <c r="IU6" s="121" t="n">
         <f aca="false">(IU10*IT6)</f>
         <v>0.7</v>
       </c>
-      <c r="IV6" s="89" t="n">
+      <c r="IV6" s="88" t="n">
         <f aca="false">(IV10*IT6)</f>
         <v>1.4</v>
       </c>
-      <c r="IW6" s="123" t="n">
+      <c r="IW6" s="122" t="n">
         <f aca="false">(IW10*IT6)</f>
         <v>2.1</v>
       </c>
-      <c r="IX6" s="124" t="n">
+      <c r="IX6" s="123" t="n">
         <f aca="false">(IX10*IT6)</f>
         <v>2.8</v>
       </c>
-      <c r="IY6" s="125" t="n">
+      <c r="IY6" s="124" t="n">
         <f aca="false">(IY10*IT6)</f>
         <v>3.5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="46.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="103" t="n">
+      <c r="A7" s="102" t="n">
         <f aca="false">A6+1</f>
         <v>3</v>
       </c>
-      <c r="B7" s="104" t="s">
-        <v>123</v>
-      </c>
-      <c r="C7" s="105" t="n">
+      <c r="B7" s="103" t="s">
+        <v>124</v>
+      </c>
+      <c r="C7" s="104" t="n">
         <v>2</v>
       </c>
-      <c r="D7" s="105" t="n">
+      <c r="D7" s="104" t="n">
         <v>4</v>
       </c>
-      <c r="E7" s="105" t="n">
+      <c r="E7" s="104" t="n">
         <f aca="false">PRODUCT(C7:D7)</f>
         <v>8</v>
       </c>
-      <c r="F7" s="104" t="s">
-        <v>124</v>
-      </c>
-      <c r="G7" s="104" t="s">
+      <c r="F7" s="103" t="s">
         <v>125</v>
       </c>
-      <c r="H7" s="105"/>
-      <c r="I7" s="105" t="s">
+      <c r="G7" s="103" t="s">
+        <v>126</v>
+      </c>
+      <c r="H7" s="104" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" s="104" t="s">
         <v>115</v>
       </c>
-      <c r="J7" s="106"/>
-      <c r="K7" s="107"/>
-      <c r="L7" s="94"/>
-      <c r="M7" s="95" t="n">
+      <c r="J7" s="105" t="s">
+        <v>116</v>
+      </c>
+      <c r="K7" s="106"/>
+      <c r="L7" s="93"/>
+      <c r="M7" s="94" t="n">
         <v>2</v>
       </c>
-      <c r="N7" s="126" t="n">
+      <c r="N7" s="125" t="n">
         <v>2</v>
       </c>
-      <c r="O7" s="127" t="n">
+      <c r="O7" s="126" t="n">
         <v>4</v>
       </c>
-      <c r="P7" s="128" t="n">
+      <c r="P7" s="127" t="n">
         <v>6</v>
       </c>
-      <c r="Q7" s="129" t="n">
+      <c r="Q7" s="128" t="n">
         <v>8</v>
       </c>
-      <c r="R7" s="97" t="n">
+      <c r="R7" s="96" t="n">
         <v>10</v>
       </c>
-      <c r="S7" s="130"/>
-      <c r="T7" s="120" t="n">
+      <c r="S7" s="129"/>
+      <c r="T7" s="119" t="n">
         <v>2</v>
       </c>
-      <c r="U7" s="131" t="s">
-        <v>126</v>
-      </c>
-      <c r="IR7" s="113"/>
-      <c r="IS7" s="114" t="s">
+      <c r="U7" s="130" t="s">
         <v>127</v>
       </c>
-      <c r="IT7" s="43" t="n">
+      <c r="IR7" s="112"/>
+      <c r="IS7" s="113" t="s">
+        <v>128</v>
+      </c>
+      <c r="IT7" s="42" t="n">
         <v>0.5</v>
       </c>
-      <c r="IU7" s="122" t="n">
+      <c r="IU7" s="121" t="n">
         <f aca="false">(IU10*IT7)</f>
         <v>0.5</v>
       </c>
-      <c r="IV7" s="124" t="n">
+      <c r="IV7" s="123" t="n">
         <f aca="false">(IV10*IT7)</f>
         <v>1</v>
       </c>
-      <c r="IW7" s="89" t="n">
+      <c r="IW7" s="88" t="n">
         <f aca="false">(IW10*IT7)</f>
         <v>1.5</v>
       </c>
-      <c r="IX7" s="89" t="n">
+      <c r="IX7" s="88" t="n">
         <f aca="false">(IX10*IT7)</f>
         <v>2</v>
       </c>
-      <c r="IY7" s="132" t="n">
+      <c r="IY7" s="131" t="n">
         <f aca="false">(IY10*IT7)</f>
         <v>2.5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="55.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="103" t="n">
+      <c r="A8" s="102" t="n">
         <f aca="false">A7+1</f>
         <v>4</v>
       </c>
-      <c r="B8" s="104" t="s">
-        <v>128</v>
-      </c>
-      <c r="C8" s="105" t="n">
+      <c r="B8" s="103" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" s="104" t="n">
         <v>5</v>
       </c>
-      <c r="D8" s="105" t="n">
+      <c r="D8" s="104" t="n">
         <v>2</v>
       </c>
-      <c r="E8" s="105" t="n">
+      <c r="E8" s="104" t="n">
         <f aca="false">PRODUCT(C8:D8)</f>
         <v>10</v>
       </c>
-      <c r="F8" s="104" t="s">
-        <v>129</v>
-      </c>
-      <c r="G8" s="104" t="s">
+      <c r="F8" s="103" t="s">
         <v>130</v>
       </c>
-      <c r="H8" s="105" t="s">
+      <c r="G8" s="103" t="s">
+        <v>131</v>
+      </c>
+      <c r="H8" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="105" t="s">
+      <c r="I8" s="104" t="s">
         <v>115</v>
       </c>
-      <c r="J8" s="106"/>
-      <c r="K8" s="107"/>
-      <c r="L8" s="94"/>
-      <c r="M8" s="95" t="n">
+      <c r="J8" s="105" t="s">
+        <v>116</v>
+      </c>
+      <c r="K8" s="106"/>
+      <c r="L8" s="93"/>
+      <c r="M8" s="94" t="n">
         <v>1</v>
       </c>
-      <c r="N8" s="133" t="n">
+      <c r="N8" s="132" t="n">
         <v>1</v>
       </c>
-      <c r="O8" s="134" t="n">
+      <c r="O8" s="133" t="n">
         <v>2</v>
       </c>
-      <c r="P8" s="135" t="n">
+      <c r="P8" s="134" t="n">
         <v>3</v>
       </c>
-      <c r="Q8" s="136" t="n">
+      <c r="Q8" s="135" t="n">
         <v>4</v>
       </c>
-      <c r="R8" s="119" t="n">
+      <c r="R8" s="118" t="n">
         <v>5</v>
       </c>
-      <c r="S8" s="101"/>
-      <c r="T8" s="120" t="n">
+      <c r="S8" s="100"/>
+      <c r="T8" s="119" t="n">
         <v>3</v>
       </c>
-      <c r="U8" s="131" t="s">
-        <v>131</v>
-      </c>
-      <c r="IR8" s="113"/>
-      <c r="IS8" s="114" t="s">
+      <c r="U8" s="130" t="s">
         <v>132</v>
       </c>
-      <c r="IT8" s="43" t="n">
+      <c r="IR8" s="112"/>
+      <c r="IS8" s="113" t="s">
+        <v>133</v>
+      </c>
+      <c r="IT8" s="42" t="n">
         <v>0.3</v>
       </c>
-      <c r="IU8" s="137" t="n">
+      <c r="IU8" s="136" t="n">
         <f aca="false">(IU10*IT8)</f>
         <v>0.3</v>
       </c>
-      <c r="IV8" s="123" t="n">
+      <c r="IV8" s="122" t="n">
         <f aca="false">(IV10*IT8)</f>
         <v>0.6</v>
       </c>
-      <c r="IW8" s="89" t="n">
+      <c r="IW8" s="88" t="n">
         <f aca="false">(IW10*IT8)</f>
         <v>0.9</v>
       </c>
-      <c r="IX8" s="89" t="n">
+      <c r="IX8" s="88" t="n">
         <f aca="false">(IX10*IT8)</f>
         <v>1.2</v>
       </c>
-      <c r="IY8" s="125" t="n">
+      <c r="IY8" s="124" t="n">
         <f aca="false">(IY10*IT8)</f>
         <v>1.5</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="57.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="103" t="n">
+      <c r="A9" s="102" t="n">
         <f aca="false">A8+1</f>
         <v>5</v>
       </c>
-      <c r="B9" s="104" t="s">
-        <v>133</v>
-      </c>
-      <c r="C9" s="105" t="n">
+      <c r="B9" s="103" t="s">
+        <v>134</v>
+      </c>
+      <c r="C9" s="104" t="n">
         <v>3</v>
       </c>
-      <c r="D9" s="105" t="n">
+      <c r="D9" s="104" t="n">
         <v>1</v>
       </c>
-      <c r="E9" s="105" t="n">
+      <c r="E9" s="104" t="n">
         <f aca="false">PRODUCT(C9:D9)</f>
         <v>3</v>
       </c>
-      <c r="F9" s="104" t="s">
-        <v>134</v>
-      </c>
-      <c r="G9" s="104" t="s">
+      <c r="F9" s="103" t="s">
         <v>135</v>
       </c>
-      <c r="H9" s="105" t="s">
+      <c r="G9" s="103" t="s">
+        <v>136</v>
+      </c>
+      <c r="H9" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="I9" s="105" t="s">
+      <c r="I9" s="104" t="s">
         <v>115</v>
       </c>
-      <c r="J9" s="106"/>
-      <c r="K9" s="107"/>
-      <c r="L9" s="95"/>
-      <c r="M9" s="138"/>
-      <c r="N9" s="139" t="n">
+      <c r="J9" s="105" t="s">
+        <v>116</v>
+      </c>
+      <c r="K9" s="106"/>
+      <c r="L9" s="94"/>
+      <c r="M9" s="137"/>
+      <c r="N9" s="138" t="n">
         <v>1</v>
       </c>
-      <c r="O9" s="140" t="n">
+      <c r="O9" s="139" t="n">
         <v>2</v>
       </c>
-      <c r="P9" s="139" t="n">
+      <c r="P9" s="138" t="n">
         <v>3</v>
       </c>
-      <c r="Q9" s="140" t="n">
+      <c r="Q9" s="139" t="n">
         <v>4</v>
       </c>
-      <c r="R9" s="139" t="n">
+      <c r="R9" s="138" t="n">
         <v>5</v>
       </c>
-      <c r="S9" s="141"/>
-      <c r="T9" s="120" t="n">
+      <c r="S9" s="140"/>
+      <c r="T9" s="119" t="n">
         <v>4</v>
       </c>
-      <c r="U9" s="131" t="s">
-        <v>136</v>
-      </c>
-      <c r="IR9" s="113"/>
-      <c r="IS9" s="114" t="s">
-        <v>127</v>
-      </c>
-      <c r="IT9" s="142" t="n">
+      <c r="U9" s="130" t="s">
+        <v>137</v>
+      </c>
+      <c r="IR9" s="112"/>
+      <c r="IS9" s="113" t="s">
+        <v>128</v>
+      </c>
+      <c r="IT9" s="141" t="n">
         <v>0.1</v>
       </c>
-      <c r="IU9" s="124" t="n">
+      <c r="IU9" s="123" t="n">
         <f aca="false">(IU10*IT9)</f>
         <v>0.1</v>
       </c>
-      <c r="IV9" s="143" t="n">
+      <c r="IV9" s="142" t="n">
         <f aca="false">(IV10*IT9)</f>
         <v>0.2</v>
       </c>
-      <c r="IW9" s="144" t="n">
+      <c r="IW9" s="143" t="n">
         <f aca="false">(IW10*IU9)</f>
         <v>0.3</v>
       </c>
-      <c r="IX9" s="144" t="n">
+      <c r="IX9" s="143" t="n">
         <f aca="false">(IX10*IT9)</f>
         <v>0.4</v>
       </c>
-      <c r="IY9" s="145" t="n">
+      <c r="IY9" s="144" t="n">
         <f aca="false">(IY10*IT9)</f>
         <v>0.5</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="57.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="146" t="n">
+      <c r="A10" s="145" t="n">
         <f aca="false">A9+1</f>
         <v>6</v>
       </c>
-      <c r="B10" s="104"/>
-      <c r="C10" s="105"/>
-      <c r="D10" s="105"/>
-      <c r="E10" s="147" t="n">
+      <c r="B10" s="103"/>
+      <c r="C10" s="104"/>
+      <c r="D10" s="104"/>
+      <c r="E10" s="146" t="n">
         <f aca="false">PRODUCT(C10:D10)</f>
         <v>0</v>
       </c>
-      <c r="F10" s="148"/>
-      <c r="G10" s="104"/>
-      <c r="H10" s="105"/>
-      <c r="I10" s="147"/>
-      <c r="J10" s="149"/>
-      <c r="L10" s="95"/>
-      <c r="M10" s="138"/>
-      <c r="N10" s="150" t="s">
+      <c r="F10" s="147"/>
+      <c r="G10" s="103"/>
+      <c r="H10" s="104"/>
+      <c r="I10" s="146"/>
+      <c r="J10" s="148"/>
+      <c r="L10" s="94"/>
+      <c r="M10" s="137"/>
+      <c r="N10" s="149" t="s">
         <v>104</v>
       </c>
-      <c r="O10" s="150"/>
-      <c r="P10" s="150"/>
-      <c r="Q10" s="150"/>
-      <c r="R10" s="150"/>
-      <c r="S10" s="151"/>
-      <c r="T10" s="120" t="n">
+      <c r="O10" s="149"/>
+      <c r="P10" s="149"/>
+      <c r="Q10" s="149"/>
+      <c r="R10" s="149"/>
+      <c r="S10" s="150"/>
+      <c r="T10" s="119" t="n">
         <v>5</v>
       </c>
-      <c r="U10" s="131" t="s">
-        <v>137</v>
-      </c>
-      <c r="IR10" s="152"/>
-      <c r="IS10" s="89"/>
-      <c r="IT10" s="114"/>
-      <c r="IU10" s="43" t="n">
+      <c r="U10" s="130" t="s">
+        <v>138</v>
+      </c>
+      <c r="IR10" s="151"/>
+      <c r="IS10" s="88"/>
+      <c r="IT10" s="113"/>
+      <c r="IU10" s="42" t="n">
         <v>1</v>
       </c>
-      <c r="IV10" s="43" t="n">
+      <c r="IV10" s="42" t="n">
         <v>2</v>
       </c>
-      <c r="IW10" s="43" t="n">
+      <c r="IW10" s="42" t="n">
         <v>3</v>
       </c>
-      <c r="IX10" s="43" t="n">
+      <c r="IX10" s="42" t="n">
         <v>4</v>
       </c>
-      <c r="IY10" s="153" t="n">
+      <c r="IY10" s="152" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="146" t="n">
+      <c r="A11" s="145" t="n">
         <f aca="false">A10+1</f>
         <v>7</v>
       </c>
-      <c r="B11" s="104"/>
-      <c r="C11" s="105"/>
-      <c r="D11" s="105"/>
-      <c r="E11" s="147" t="n">
+      <c r="B11" s="103"/>
+      <c r="C11" s="104"/>
+      <c r="D11" s="104"/>
+      <c r="E11" s="146" t="n">
         <f aca="false">PRODUCT(C11:D11)</f>
         <v>0</v>
       </c>
-      <c r="F11" s="148"/>
-      <c r="G11" s="104"/>
-      <c r="H11" s="105"/>
-      <c r="I11" s="147"/>
-      <c r="J11" s="149"/>
-      <c r="L11" s="154"/>
-      <c r="M11" s="151"/>
-      <c r="N11" s="154"/>
-      <c r="O11" s="151"/>
-      <c r="P11" s="151"/>
-      <c r="Q11" s="151"/>
-      <c r="R11" s="151"/>
-      <c r="S11" s="151"/>
-      <c r="T11" s="111" t="s">
-        <v>116</v>
-      </c>
-      <c r="U11" s="155" t="s">
+      <c r="F11" s="147"/>
+      <c r="G11" s="103"/>
+      <c r="H11" s="104"/>
+      <c r="I11" s="146"/>
+      <c r="J11" s="148"/>
+      <c r="L11" s="153"/>
+      <c r="M11" s="150"/>
+      <c r="N11" s="153"/>
+      <c r="O11" s="150"/>
+      <c r="P11" s="150"/>
+      <c r="Q11" s="150"/>
+      <c r="R11" s="150"/>
+      <c r="S11" s="150"/>
+      <c r="T11" s="110" t="s">
+        <v>117</v>
+      </c>
+      <c r="U11" s="154" t="s">
         <v>105</v>
       </c>
-      <c r="IR11" s="152"/>
-      <c r="IS11" s="89"/>
-      <c r="IT11" s="89"/>
-      <c r="IU11" s="114" t="s">
-        <v>127</v>
-      </c>
-      <c r="IV11" s="114" t="s">
-        <v>132</v>
-      </c>
-      <c r="IW11" s="114" t="s">
-        <v>138</v>
-      </c>
-      <c r="IX11" s="114" t="s">
-        <v>122</v>
-      </c>
-      <c r="IY11" s="156" t="s">
-        <v>117</v>
+      <c r="IR11" s="151"/>
+      <c r="IS11" s="88"/>
+      <c r="IT11" s="88"/>
+      <c r="IU11" s="113" t="s">
+        <v>128</v>
+      </c>
+      <c r="IV11" s="113" t="s">
+        <v>133</v>
+      </c>
+      <c r="IW11" s="113" t="s">
+        <v>139</v>
+      </c>
+      <c r="IX11" s="113" t="s">
+        <v>123</v>
+      </c>
+      <c r="IY11" s="155" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="146" t="n">
+      <c r="A12" s="145" t="n">
         <f aca="false">A11+1</f>
         <v>8</v>
       </c>
-      <c r="B12" s="104"/>
-      <c r="C12" s="105"/>
-      <c r="D12" s="105"/>
-      <c r="E12" s="147" t="n">
+      <c r="B12" s="103"/>
+      <c r="C12" s="104"/>
+      <c r="D12" s="104"/>
+      <c r="E12" s="146" t="n">
         <f aca="false">PRODUCT(C12:D12)</f>
         <v>0</v>
       </c>
-      <c r="F12" s="148"/>
-      <c r="G12" s="104"/>
-      <c r="H12" s="105"/>
-      <c r="I12" s="147"/>
-      <c r="J12" s="149"/>
-      <c r="L12" s="154"/>
-      <c r="M12" s="151"/>
-      <c r="N12" s="151"/>
-      <c r="O12" s="151"/>
-      <c r="P12" s="151"/>
-      <c r="Q12" s="151"/>
-      <c r="R12" s="151"/>
-      <c r="S12" s="151"/>
-      <c r="T12" s="120" t="n">
+      <c r="F12" s="147"/>
+      <c r="G12" s="103"/>
+      <c r="H12" s="104"/>
+      <c r="I12" s="146"/>
+      <c r="J12" s="148"/>
+      <c r="L12" s="153"/>
+      <c r="M12" s="150"/>
+      <c r="N12" s="150"/>
+      <c r="O12" s="150"/>
+      <c r="P12" s="150"/>
+      <c r="Q12" s="150"/>
+      <c r="R12" s="150"/>
+      <c r="S12" s="150"/>
+      <c r="T12" s="119" t="n">
         <v>1</v>
       </c>
-      <c r="U12" s="157" t="s">
-        <v>139</v>
-      </c>
-      <c r="IR12" s="152"/>
-      <c r="IS12" s="89"/>
-      <c r="IT12" s="43"/>
-      <c r="IU12" s="158" t="s">
+      <c r="U12" s="156" t="s">
+        <v>140</v>
+      </c>
+      <c r="IR12" s="151"/>
+      <c r="IS12" s="88"/>
+      <c r="IT12" s="42"/>
+      <c r="IU12" s="157" t="s">
         <v>104</v>
       </c>
-      <c r="IV12" s="158"/>
-      <c r="IW12" s="158"/>
-      <c r="IX12" s="158"/>
-      <c r="IY12" s="158"/>
+      <c r="IV12" s="157"/>
+      <c r="IW12" s="157"/>
+      <c r="IX12" s="157"/>
+      <c r="IY12" s="157"/>
     </row>
     <row r="13" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="146" t="n">
+      <c r="A13" s="145" t="n">
         <f aca="false">A12+1</f>
         <v>9</v>
       </c>
-      <c r="B13" s="104"/>
-      <c r="C13" s="105"/>
-      <c r="D13" s="105"/>
-      <c r="E13" s="147" t="n">
+      <c r="B13" s="103"/>
+      <c r="C13" s="104"/>
+      <c r="D13" s="104"/>
+      <c r="E13" s="146" t="n">
         <f aca="false">PRODUCT(C13:D13)</f>
         <v>0</v>
       </c>
-      <c r="F13" s="148"/>
-      <c r="G13" s="104"/>
-      <c r="H13" s="105"/>
-      <c r="I13" s="147"/>
-      <c r="J13" s="149"/>
-      <c r="L13" s="154"/>
-      <c r="M13" s="151"/>
-      <c r="N13" s="151"/>
-      <c r="O13" s="151"/>
-      <c r="P13" s="151"/>
-      <c r="Q13" s="151"/>
-      <c r="R13" s="151"/>
-      <c r="S13" s="151"/>
-      <c r="T13" s="120" t="n">
+      <c r="F13" s="147"/>
+      <c r="G13" s="103"/>
+      <c r="H13" s="104"/>
+      <c r="I13" s="146"/>
+      <c r="J13" s="148"/>
+      <c r="L13" s="153"/>
+      <c r="M13" s="150"/>
+      <c r="N13" s="150"/>
+      <c r="O13" s="150"/>
+      <c r="P13" s="150"/>
+      <c r="Q13" s="150"/>
+      <c r="R13" s="150"/>
+      <c r="S13" s="150"/>
+      <c r="T13" s="119" t="n">
         <v>2</v>
       </c>
-      <c r="U13" s="121" t="s">
-        <v>140</v>
-      </c>
-      <c r="IR13" s="152"/>
-      <c r="IS13" s="89"/>
-      <c r="IT13" s="89"/>
-      <c r="IU13" s="89"/>
-      <c r="IV13" s="89"/>
-      <c r="IW13" s="89"/>
-      <c r="IX13" s="89"/>
-      <c r="IY13" s="132"/>
+      <c r="U13" s="120" t="s">
+        <v>141</v>
+      </c>
+      <c r="IR13" s="151"/>
+      <c r="IS13" s="88"/>
+      <c r="IT13" s="88"/>
+      <c r="IU13" s="88"/>
+      <c r="IV13" s="88"/>
+      <c r="IW13" s="88"/>
+      <c r="IX13" s="88"/>
+      <c r="IY13" s="131"/>
     </row>
     <row r="14" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="146" t="n">
+      <c r="A14" s="145" t="n">
         <f aca="false">A13+1</f>
         <v>10</v>
       </c>
-      <c r="B14" s="104"/>
-      <c r="C14" s="105"/>
-      <c r="D14" s="105"/>
-      <c r="E14" s="147" t="n">
+      <c r="B14" s="103"/>
+      <c r="C14" s="104"/>
+      <c r="D14" s="104"/>
+      <c r="E14" s="146" t="n">
         <f aca="false">PRODUCT(C14:D14)</f>
         <v>0</v>
       </c>
-      <c r="F14" s="148"/>
-      <c r="G14" s="104"/>
-      <c r="H14" s="105"/>
-      <c r="I14" s="147"/>
-      <c r="J14" s="149"/>
-      <c r="L14" s="154"/>
-      <c r="M14" s="151"/>
-      <c r="N14" s="151"/>
-      <c r="O14" s="151"/>
-      <c r="P14" s="151"/>
-      <c r="Q14" s="151"/>
-      <c r="R14" s="151"/>
-      <c r="S14" s="151"/>
-      <c r="T14" s="120" t="n">
+      <c r="F14" s="147"/>
+      <c r="G14" s="103"/>
+      <c r="H14" s="104"/>
+      <c r="I14" s="146"/>
+      <c r="J14" s="148"/>
+      <c r="L14" s="153"/>
+      <c r="M14" s="150"/>
+      <c r="N14" s="150"/>
+      <c r="O14" s="150"/>
+      <c r="P14" s="150"/>
+      <c r="Q14" s="150"/>
+      <c r="R14" s="150"/>
+      <c r="S14" s="150"/>
+      <c r="T14" s="119" t="n">
         <v>3</v>
       </c>
-      <c r="U14" s="131" t="s">
-        <v>141</v>
-      </c>
-      <c r="IR14" s="152"/>
-      <c r="IS14" s="89"/>
-      <c r="IT14" s="42"/>
-      <c r="IU14" s="42"/>
-      <c r="IV14" s="42"/>
-      <c r="IW14" s="42"/>
-      <c r="IX14" s="42"/>
-      <c r="IY14" s="159"/>
+      <c r="U14" s="130" t="s">
+        <v>142</v>
+      </c>
+      <c r="IR14" s="151"/>
+      <c r="IS14" s="88"/>
+      <c r="IT14" s="41"/>
+      <c r="IU14" s="41"/>
+      <c r="IV14" s="41"/>
+      <c r="IW14" s="41"/>
+      <c r="IX14" s="41"/>
+      <c r="IY14" s="158"/>
     </row>
     <row r="15" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="146" t="n">
+      <c r="A15" s="145" t="n">
         <f aca="false">A14+1</f>
         <v>11</v>
       </c>
-      <c r="B15" s="104"/>
-      <c r="C15" s="105"/>
-      <c r="D15" s="105"/>
-      <c r="E15" s="147" t="n">
+      <c r="B15" s="103"/>
+      <c r="C15" s="104"/>
+      <c r="D15" s="104"/>
+      <c r="E15" s="146" t="n">
         <f aca="false">PRODUCT(C15:D15)</f>
         <v>0</v>
       </c>
-      <c r="F15" s="148"/>
-      <c r="G15" s="104"/>
-      <c r="H15" s="105"/>
-      <c r="I15" s="147"/>
-      <c r="J15" s="149"/>
+      <c r="F15" s="147"/>
+      <c r="G15" s="103"/>
+      <c r="H15" s="104"/>
+      <c r="I15" s="146"/>
+      <c r="J15" s="148"/>
       <c r="L15" s="32"/>
-      <c r="M15" s="151"/>
-      <c r="N15" s="151"/>
-      <c r="O15" s="151"/>
-      <c r="P15" s="151"/>
-      <c r="Q15" s="151"/>
-      <c r="R15" s="151"/>
-      <c r="S15" s="151"/>
-      <c r="T15" s="120" t="n">
+      <c r="M15" s="150"/>
+      <c r="N15" s="150"/>
+      <c r="O15" s="150"/>
+      <c r="P15" s="150"/>
+      <c r="Q15" s="150"/>
+      <c r="R15" s="150"/>
+      <c r="S15" s="150"/>
+      <c r="T15" s="119" t="n">
         <v>4</v>
       </c>
-      <c r="U15" s="131" t="s">
-        <v>142</v>
-      </c>
-      <c r="IR15" s="160" t="s">
+      <c r="U15" s="130" t="s">
         <v>143</v>
       </c>
-      <c r="IS15" s="160"/>
-      <c r="IT15" s="42"/>
-      <c r="IU15" s="42"/>
-      <c r="IV15" s="42"/>
-      <c r="IW15" s="42"/>
-      <c r="IX15" s="42"/>
-      <c r="IY15" s="159"/>
+      <c r="IR15" s="159" t="s">
+        <v>144</v>
+      </c>
+      <c r="IS15" s="159"/>
+      <c r="IT15" s="41"/>
+      <c r="IU15" s="41"/>
+      <c r="IV15" s="41"/>
+      <c r="IW15" s="41"/>
+      <c r="IX15" s="41"/>
+      <c r="IY15" s="158"/>
     </row>
     <row r="16" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="146" t="n">
+      <c r="A16" s="145" t="n">
         <f aca="false">A15+1</f>
         <v>12</v>
       </c>
-      <c r="B16" s="104"/>
-      <c r="C16" s="105"/>
-      <c r="D16" s="105"/>
-      <c r="E16" s="147" t="n">
+      <c r="B16" s="103"/>
+      <c r="C16" s="104"/>
+      <c r="D16" s="104"/>
+      <c r="E16" s="146" t="n">
         <f aca="false">PRODUCT(C16:D16)</f>
         <v>0</v>
       </c>
-      <c r="F16" s="148"/>
-      <c r="G16" s="104"/>
-      <c r="H16" s="105"/>
-      <c r="I16" s="147"/>
-      <c r="J16" s="149"/>
+      <c r="F16" s="147"/>
+      <c r="G16" s="103"/>
+      <c r="H16" s="104"/>
+      <c r="I16" s="146"/>
+      <c r="J16" s="148"/>
       <c r="L16" s="32"/>
-      <c r="M16" s="151"/>
-      <c r="N16" s="151"/>
-      <c r="O16" s="151"/>
-      <c r="P16" s="151"/>
-      <c r="Q16" s="151"/>
-      <c r="R16" s="151"/>
-      <c r="S16" s="151"/>
-      <c r="T16" s="120" t="n">
+      <c r="M16" s="150"/>
+      <c r="N16" s="150"/>
+      <c r="O16" s="150"/>
+      <c r="P16" s="150"/>
+      <c r="Q16" s="150"/>
+      <c r="R16" s="150"/>
+      <c r="S16" s="150"/>
+      <c r="T16" s="119" t="n">
         <v>5</v>
       </c>
-      <c r="U16" s="157" t="s">
-        <v>144</v>
-      </c>
-      <c r="IR16" s="152" t="s">
+      <c r="U16" s="156" t="s">
         <v>145</v>
       </c>
-      <c r="IS16" s="161"/>
-      <c r="IT16" s="42"/>
-      <c r="IU16" s="162" t="s">
+      <c r="IR16" s="151" t="s">
         <v>146</v>
       </c>
-      <c r="IV16" s="162"/>
-      <c r="IW16" s="162"/>
-      <c r="IX16" s="162"/>
-      <c r="IY16" s="162"/>
+      <c r="IS16" s="160"/>
+      <c r="IT16" s="41"/>
+      <c r="IU16" s="161" t="s">
+        <v>147</v>
+      </c>
+      <c r="IV16" s="161"/>
+      <c r="IW16" s="161"/>
+      <c r="IX16" s="161"/>
+      <c r="IY16" s="161"/>
     </row>
     <row r="17" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="146" t="n">
+      <c r="A17" s="145" t="n">
         <f aca="false">A16+1</f>
         <v>13</v>
       </c>
-      <c r="B17" s="104"/>
-      <c r="C17" s="105"/>
-      <c r="D17" s="105"/>
-      <c r="E17" s="147" t="n">
+      <c r="B17" s="103"/>
+      <c r="C17" s="104"/>
+      <c r="D17" s="104"/>
+      <c r="E17" s="146" t="n">
         <f aca="false">PRODUCT(C17:D17)</f>
         <v>0</v>
       </c>
-      <c r="F17" s="148"/>
-      <c r="G17" s="104"/>
-      <c r="H17" s="105"/>
-      <c r="I17" s="147"/>
-      <c r="J17" s="149"/>
+      <c r="F17" s="147"/>
+      <c r="G17" s="103"/>
+      <c r="H17" s="104"/>
+      <c r="I17" s="146"/>
+      <c r="J17" s="148"/>
       <c r="L17" s="32"/>
-      <c r="M17" s="151"/>
-      <c r="N17" s="151"/>
-      <c r="O17" s="151"/>
-      <c r="P17" s="151"/>
-      <c r="Q17" s="151"/>
-      <c r="R17" s="151"/>
-      <c r="S17" s="151"/>
-      <c r="T17" s="163"/>
-      <c r="U17" s="155" t="s">
+      <c r="M17" s="150"/>
+      <c r="N17" s="150"/>
+      <c r="O17" s="150"/>
+      <c r="P17" s="150"/>
+      <c r="Q17" s="150"/>
+      <c r="R17" s="150"/>
+      <c r="S17" s="150"/>
+      <c r="T17" s="162"/>
+      <c r="U17" s="154" t="s">
         <v>106</v>
       </c>
-      <c r="IR17" s="152" t="s">
-        <v>147</v>
-      </c>
-      <c r="IS17" s="161"/>
-      <c r="IT17" s="42"/>
-      <c r="IU17" s="162" t="s">
+      <c r="IR17" s="151" t="s">
         <v>148</v>
       </c>
-      <c r="IV17" s="162"/>
-      <c r="IW17" s="162"/>
-      <c r="IX17" s="162"/>
-      <c r="IY17" s="162"/>
+      <c r="IS17" s="160"/>
+      <c r="IT17" s="41"/>
+      <c r="IU17" s="161" t="s">
+        <v>149</v>
+      </c>
+      <c r="IV17" s="161"/>
+      <c r="IW17" s="161"/>
+      <c r="IX17" s="161"/>
+      <c r="IY17" s="161"/>
     </row>
     <row r="18" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="146" t="n">
+      <c r="A18" s="145" t="n">
         <f aca="false">A17+1</f>
         <v>14</v>
       </c>
-      <c r="B18" s="104"/>
-      <c r="C18" s="105"/>
-      <c r="D18" s="105"/>
-      <c r="E18" s="147" t="n">
+      <c r="B18" s="103"/>
+      <c r="C18" s="104"/>
+      <c r="D18" s="104"/>
+      <c r="E18" s="146" t="n">
         <f aca="false">PRODUCT(C18:D18)</f>
         <v>0</v>
       </c>
-      <c r="F18" s="148"/>
-      <c r="G18" s="104"/>
-      <c r="H18" s="105"/>
-      <c r="I18" s="147"/>
-      <c r="J18" s="149"/>
+      <c r="F18" s="147"/>
+      <c r="G18" s="103"/>
+      <c r="H18" s="104"/>
+      <c r="I18" s="146"/>
+      <c r="J18" s="148"/>
       <c r="L18" s="32"/>
-      <c r="M18" s="151"/>
-      <c r="N18" s="151"/>
-      <c r="O18" s="151"/>
-      <c r="P18" s="151"/>
-      <c r="Q18" s="151"/>
-      <c r="R18" s="151"/>
-      <c r="S18" s="151"/>
-      <c r="T18" s="164"/>
-      <c r="U18" s="131" t="s">
+      <c r="M18" s="150"/>
+      <c r="N18" s="150"/>
+      <c r="O18" s="150"/>
+      <c r="P18" s="150"/>
+      <c r="Q18" s="150"/>
+      <c r="R18" s="150"/>
+      <c r="S18" s="150"/>
+      <c r="T18" s="163"/>
+      <c r="U18" s="130" t="s">
+        <v>150</v>
+      </c>
+      <c r="IR18" s="151" t="s">
+        <v>151</v>
+      </c>
+      <c r="IS18" s="160"/>
+      <c r="IT18" s="41"/>
+      <c r="IU18" s="161" t="s">
         <v>149</v>
       </c>
-      <c r="IR18" s="152" t="s">
-        <v>150</v>
-      </c>
-      <c r="IS18" s="161"/>
-      <c r="IT18" s="42"/>
-      <c r="IU18" s="162" t="s">
-        <v>148</v>
-      </c>
-      <c r="IV18" s="162"/>
-      <c r="IW18" s="162"/>
-      <c r="IX18" s="162"/>
-      <c r="IY18" s="162"/>
+      <c r="IV18" s="161"/>
+      <c r="IW18" s="161"/>
+      <c r="IX18" s="161"/>
+      <c r="IY18" s="161"/>
     </row>
     <row r="19" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="146" t="n">
+      <c r="A19" s="145" t="n">
         <f aca="false">A18+1</f>
         <v>15</v>
       </c>
-      <c r="B19" s="104"/>
-      <c r="C19" s="105"/>
-      <c r="D19" s="105"/>
-      <c r="E19" s="147" t="n">
+      <c r="B19" s="103"/>
+      <c r="C19" s="104"/>
+      <c r="D19" s="104"/>
+      <c r="E19" s="146" t="n">
         <f aca="false">PRODUCT(C19:D19)</f>
         <v>0</v>
       </c>
-      <c r="F19" s="148"/>
-      <c r="G19" s="104"/>
-      <c r="H19" s="105"/>
-      <c r="I19" s="147"/>
-      <c r="J19" s="149"/>
+      <c r="F19" s="147"/>
+      <c r="G19" s="103"/>
+      <c r="H19" s="104"/>
+      <c r="I19" s="146"/>
+      <c r="J19" s="148"/>
       <c r="L19" s="32"/>
-      <c r="M19" s="151"/>
-      <c r="N19" s="151"/>
-      <c r="O19" s="151"/>
-      <c r="P19" s="151"/>
-      <c r="Q19" s="151"/>
-      <c r="R19" s="151"/>
-      <c r="S19" s="151"/>
-      <c r="T19" s="165"/>
-      <c r="U19" s="131" t="s">
-        <v>151</v>
-      </c>
-      <c r="IR19" s="166"/>
-      <c r="IS19" s="90"/>
-      <c r="IT19" s="167"/>
-      <c r="IU19" s="167"/>
-      <c r="IV19" s="167"/>
-      <c r="IW19" s="167"/>
-      <c r="IX19" s="167"/>
-      <c r="IY19" s="168"/>
+      <c r="M19" s="150"/>
+      <c r="N19" s="150"/>
+      <c r="O19" s="150"/>
+      <c r="P19" s="150"/>
+      <c r="Q19" s="150"/>
+      <c r="R19" s="150"/>
+      <c r="S19" s="150"/>
+      <c r="T19" s="164"/>
+      <c r="U19" s="130" t="s">
+        <v>152</v>
+      </c>
+      <c r="IR19" s="165"/>
+      <c r="IS19" s="89"/>
+      <c r="IT19" s="166"/>
+      <c r="IU19" s="166"/>
+      <c r="IV19" s="166"/>
+      <c r="IW19" s="166"/>
+      <c r="IX19" s="166"/>
+      <c r="IY19" s="167"/>
     </row>
     <row r="20" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="146" t="n">
+      <c r="A20" s="145" t="n">
         <f aca="false">A19+1</f>
         <v>16</v>
       </c>
-      <c r="B20" s="104"/>
-      <c r="C20" s="105"/>
-      <c r="D20" s="105"/>
-      <c r="E20" s="147" t="n">
+      <c r="B20" s="103"/>
+      <c r="C20" s="104"/>
+      <c r="D20" s="104"/>
+      <c r="E20" s="146" t="n">
         <f aca="false">PRODUCT(C20:D20)</f>
         <v>0</v>
       </c>
-      <c r="F20" s="148"/>
-      <c r="G20" s="104"/>
-      <c r="H20" s="105"/>
-      <c r="I20" s="147"/>
-      <c r="J20" s="149"/>
+      <c r="F20" s="147"/>
+      <c r="G20" s="103"/>
+      <c r="H20" s="104"/>
+      <c r="I20" s="146"/>
+      <c r="J20" s="148"/>
       <c r="L20" s="32"/>
-      <c r="M20" s="151"/>
-      <c r="N20" s="151"/>
-      <c r="O20" s="151"/>
-      <c r="P20" s="151"/>
-      <c r="Q20" s="151"/>
-      <c r="R20" s="151"/>
-      <c r="S20" s="151"/>
-      <c r="T20" s="169"/>
-      <c r="U20" s="170" t="s">
-        <v>152</v>
+      <c r="M20" s="150"/>
+      <c r="N20" s="150"/>
+      <c r="O20" s="150"/>
+      <c r="P20" s="150"/>
+      <c r="Q20" s="150"/>
+      <c r="R20" s="150"/>
+      <c r="S20" s="150"/>
+      <c r="T20" s="168"/>
+      <c r="U20" s="169" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actualización de fechas trasentrega de proyecto
</commit_message>
<xml_diff>
--- a/Proyectos/Viaticos/02. Planeación/Viaticos-PlanProyecto.xlsx
+++ b/Proyectos/Viaticos/02. Planeación/Viaticos-PlanProyecto.xlsx
@@ -2213,15 +2213,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1413000</xdr:colOff>
+      <xdr:colOff>1440000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>1080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>3910680</xdr:colOff>
+      <xdr:colOff>3937320</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>62640</xdr:rowOff>
+      <xdr:rowOff>62280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2234,8 +2234,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4194720" y="1080"/>
-          <a:ext cx="2497680" cy="823320"/>
+          <a:off x="4221720" y="1080"/>
+          <a:ext cx="2497320" cy="822960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2255,15 +2255,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>432000</xdr:colOff>
+      <xdr:colOff>459000</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>154440</xdr:rowOff>
+      <xdr:rowOff>145440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>432360</xdr:colOff>
+      <xdr:colOff>459360</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>154800</xdr:rowOff>
+      <xdr:rowOff>145800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2272,7 +2272,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8243640" y="1011600"/>
+          <a:off x="8270640" y="1002600"/>
           <a:ext cx="360" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -2298,15 +2298,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>927000</xdr:colOff>
+      <xdr:colOff>954000</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>154080</xdr:rowOff>
+      <xdr:rowOff>145080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>106200</xdr:colOff>
+      <xdr:colOff>132840</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>154440</xdr:rowOff>
+      <xdr:rowOff>145440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2315,8 +2315,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4991400" y="1011240"/>
-          <a:ext cx="5390280" cy="360"/>
+          <a:off x="5018400" y="1002240"/>
+          <a:ext cx="5389920" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2338,15 +2338,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>432000</xdr:colOff>
+      <xdr:colOff>459000</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>285840</xdr:rowOff>
+      <xdr:rowOff>276840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>432360</xdr:colOff>
+      <xdr:colOff>459360</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>286200</xdr:rowOff>
+      <xdr:rowOff>277200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2355,7 +2355,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8243640" y="5031000"/>
+          <a:off x="8270640" y="5022000"/>
           <a:ext cx="360" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -2381,15 +2381,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>927000</xdr:colOff>
+      <xdr:colOff>954000</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>152280</xdr:rowOff>
+      <xdr:rowOff>143280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>105840</xdr:colOff>
+      <xdr:colOff>132480</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>152640</xdr:rowOff>
+      <xdr:rowOff>143640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2398,8 +2398,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4991400" y="5249880"/>
-          <a:ext cx="5389920" cy="360"/>
+          <a:off x="5018400" y="5240880"/>
+          <a:ext cx="5389560" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2421,15 +2421,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1086480</xdr:colOff>
+      <xdr:colOff>1113480</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>56520</xdr:rowOff>
+      <xdr:rowOff>47520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>733320</xdr:colOff>
+      <xdr:colOff>759960</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>22680</xdr:rowOff>
+      <xdr:rowOff>13320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2442,8 +2442,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7564680" y="56520"/>
-          <a:ext cx="3444120" cy="823320"/>
+          <a:off x="7591680" y="47520"/>
+          <a:ext cx="3443760" cy="822960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2463,15 +2463,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>812880</xdr:colOff>
+      <xdr:colOff>839880</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>30600</xdr:rowOff>
+      <xdr:rowOff>21600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>338760</xdr:colOff>
+      <xdr:colOff>365400</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>853920</xdr:rowOff>
+      <xdr:rowOff>844560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2484,8 +2484,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10466640" y="30600"/>
-          <a:ext cx="3489480" cy="823320"/>
+          <a:off x="10493640" y="21600"/>
+          <a:ext cx="3489120" cy="822960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2505,15 +2505,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1070280</xdr:colOff>
+      <xdr:colOff>1097280</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>424080</xdr:colOff>
+      <xdr:colOff>450720</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>823320</xdr:rowOff>
+      <xdr:rowOff>822960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2526,8 +2526,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8555400" y="0"/>
-          <a:ext cx="3545640" cy="823320"/>
+          <a:off x="8582400" y="0"/>
+          <a:ext cx="3545280" cy="822960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2547,15 +2547,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1659600</xdr:colOff>
+      <xdr:colOff>1686600</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1834920</xdr:colOff>
+      <xdr:colOff>1861560</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>823320</xdr:rowOff>
+      <xdr:rowOff>822960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2568,8 +2568,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15034320" y="0"/>
-          <a:ext cx="3274200" cy="823320"/>
+          <a:off x="15061320" y="0"/>
+          <a:ext cx="3273840" cy="822960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2591,8 +2591,8 @@
   </sheetPr>
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C15" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2782,7 +2782,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="25"/>
       <c r="B24" s="4" t="s">
         <v>27</v>
@@ -2790,9 +2790,11 @@
       <c r="C24" s="26" t="n">
         <v>42452</v>
       </c>
-      <c r="D24" s="4"/>
-    </row>
-    <row r="25" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D24" s="26" t="n">
+        <v>42452</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="25"/>
       <c r="B25" s="4" t="s">
         <v>28</v>
@@ -2800,9 +2802,11 @@
       <c r="C25" s="26" t="n">
         <v>42457</v>
       </c>
-      <c r="D25" s="4"/>
-    </row>
-    <row r="26" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D25" s="26" t="n">
+        <v>42457</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="25"/>
       <c r="B26" s="4" t="s">
         <v>29</v>
@@ -2810,9 +2814,11 @@
       <c r="C26" s="26" t="n">
         <v>42471</v>
       </c>
-      <c r="D26" s="4"/>
-    </row>
-    <row r="27" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D26" s="26" t="n">
+        <v>42471</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="25"/>
       <c r="B27" s="4" t="s">
         <v>30</v>
@@ -2820,7 +2826,9 @@
       <c r="C27" s="26" t="n">
         <v>42475</v>
       </c>
-      <c r="D27" s="4"/>
+      <c r="D27" s="26" t="n">
+        <v>42475</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="4"/>

</xml_diff>

<commit_message>
Cierre viaticos cambios plan de proyecto
</commit_message>
<xml_diff>
--- a/Proyectos/Viaticos/02. Planeación/Viaticos-PlanProyecto.xlsx
+++ b/Proyectos/Viaticos/02. Planeación/Viaticos-PlanProyecto.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Generales" sheetId="1" state="visible" r:id="rId2"/>
@@ -2216,15 +2216,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1467000</xdr:colOff>
+      <xdr:colOff>1494000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>1080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>3963960</xdr:colOff>
+      <xdr:colOff>3990600</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>61920</xdr:rowOff>
+      <xdr:rowOff>61560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2237,8 +2237,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4248720" y="1080"/>
-          <a:ext cx="2496960" cy="822600"/>
+          <a:off x="4275720" y="1080"/>
+          <a:ext cx="2496600" cy="822240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2258,15 +2258,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>486000</xdr:colOff>
+      <xdr:colOff>513000</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>136440</xdr:rowOff>
+      <xdr:rowOff>127440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>486360</xdr:colOff>
+      <xdr:colOff>513360</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>136800</xdr:rowOff>
+      <xdr:rowOff>127800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2275,7 +2275,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8297640" y="993600"/>
+          <a:off x="8324640" y="984600"/>
           <a:ext cx="360" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -2301,15 +2301,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>981000</xdr:colOff>
+      <xdr:colOff>1008000</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>136080</xdr:rowOff>
+      <xdr:rowOff>127080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>159480</xdr:colOff>
+      <xdr:colOff>186120</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>136440</xdr:rowOff>
+      <xdr:rowOff>127440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2318,8 +2318,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5045400" y="993240"/>
-          <a:ext cx="5389560" cy="360"/>
+          <a:off x="5072400" y="984240"/>
+          <a:ext cx="5389200" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2341,15 +2341,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>486000</xdr:colOff>
+      <xdr:colOff>513000</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>267840</xdr:rowOff>
+      <xdr:rowOff>258840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>486360</xdr:colOff>
+      <xdr:colOff>513360</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>268200</xdr:rowOff>
+      <xdr:rowOff>259200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2358,7 +2358,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8297640" y="5013000"/>
+          <a:off x="8324640" y="5004000"/>
           <a:ext cx="360" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -2384,15 +2384,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>981000</xdr:colOff>
+      <xdr:colOff>1008000</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>134280</xdr:rowOff>
+      <xdr:rowOff>125280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>159120</xdr:colOff>
+      <xdr:colOff>185760</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>134640</xdr:rowOff>
+      <xdr:rowOff>125640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2401,8 +2401,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5045400" y="5231880"/>
-          <a:ext cx="5389200" cy="360"/>
+          <a:off x="5072400" y="5222880"/>
+          <a:ext cx="5388840" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2424,15 +2424,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1140480</xdr:colOff>
+      <xdr:colOff>1167480</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>38520</xdr:rowOff>
+      <xdr:rowOff>29520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>786600</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>3960</xdr:rowOff>
+      <xdr:colOff>813240</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>851760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2445,8 +2445,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7618680" y="38520"/>
-          <a:ext cx="3443400" cy="822600"/>
+          <a:off x="7645680" y="29520"/>
+          <a:ext cx="3443040" cy="822240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2466,15 +2466,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>866880</xdr:colOff>
+      <xdr:colOff>893880</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>12600</xdr:rowOff>
+      <xdr:rowOff>3600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>392040</xdr:colOff>
+      <xdr:colOff>418680</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>835200</xdr:rowOff>
+      <xdr:rowOff>825840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2487,8 +2487,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10520640" y="12600"/>
-          <a:ext cx="3488760" cy="822600"/>
+          <a:off x="10547640" y="3600"/>
+          <a:ext cx="3488400" cy="822240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2508,15 +2508,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1124280</xdr:colOff>
+      <xdr:colOff>1151280</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>477360</xdr:colOff>
+      <xdr:colOff>504000</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>822600</xdr:rowOff>
+      <xdr:rowOff>822240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2529,8 +2529,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8609400" y="0"/>
-          <a:ext cx="3544920" cy="822600"/>
+          <a:off x="8636400" y="0"/>
+          <a:ext cx="3544560" cy="822240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2550,15 +2550,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1713960</xdr:colOff>
+      <xdr:colOff>1740960</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1888560</xdr:colOff>
+      <xdr:colOff>1915200</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>822600</xdr:rowOff>
+      <xdr:rowOff>822240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2571,8 +2571,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15088680" y="0"/>
-          <a:ext cx="3273480" cy="822600"/>
+          <a:off x="15115680" y="0"/>
+          <a:ext cx="3273120" cy="822240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2594,8 +2594,8 @@
   </sheetPr>
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C15" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C15" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2821,7 +2821,7 @@
         <v>42471</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="25"/>
       <c r="B27" s="4" t="s">
         <v>30</v>
@@ -2830,7 +2830,7 @@
         <v>42475</v>
       </c>
       <c r="D27" s="26" t="n">
-        <v>42475</v>
+        <v>42478</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3846,8 +3846,8 @@
   </sheetPr>
   <dimension ref="A1:IZ20"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I6" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K7" activeCellId="0" sqref="K7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C6" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>

</xml_diff>